<commit_message>
-Fix missing connection -Add TVS -Update the logo -Fix clearence and soldermask
</commit_message>
<xml_diff>
--- a/Released/BOM/H08R6.xlsx
+++ b/Released/BOM/H08R6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H08R6x-Hardware\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC85A1A5-2A0C-4857-A3EC-BD707B6148C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB5EB02-3C36-441B-8120-BB89B7779B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="114">
   <si>
     <t>Description</t>
   </si>
@@ -164,21 +164,12 @@
     <t>U2</t>
   </si>
   <si>
-    <t>Ferrite Beads Multi-Layer 30Ohm 25% 100MHz 1.5A 50mOhm DCR 0603</t>
-  </si>
-  <si>
     <t>TDK</t>
   </si>
   <si>
     <t>https://octopart.com/vlms1300-gs08-vishay-21709201?r=sp&amp;s=_gcP4_q8T1SC6PJQPTQ9yA</t>
   </si>
   <si>
-    <t>MPZ1608S601ATD25</t>
-  </si>
-  <si>
-    <t>https://octopart.com/search?q=MPZ1608S601ATD25&amp;currency=USD&amp;specs=0</t>
-  </si>
-  <si>
     <t>PCB Header, Unshrouded, Thru 02 Straight Header, .101, AMPMODU Mod II Series</t>
   </si>
   <si>
@@ -224,18 +215,6 @@
     <t>https://octopart.com/grm188r61a105ka61j-murata-9221870?r=sp</t>
   </si>
   <si>
-    <t>Tantalum Capacitors - Polymer 4.7uF 10V 20% 0603 ESR=500 mOhm</t>
-  </si>
-  <si>
-    <t>F381A475MMA</t>
-  </si>
-  <si>
-    <t>KYOCERA AVX</t>
-  </si>
-  <si>
-    <t>https://octopart.com/f381a475mma-kyocera+avx-122115684?r=sp</t>
-  </si>
-  <si>
     <t>C1, C3, C5, C6, C8, C9, C10, C14, C15, C16, C17</t>
   </si>
   <si>
@@ -245,12 +224,6 @@
     <t>CAP CER 1UF 10V X5R 0402</t>
   </si>
   <si>
-    <t xml:space="preserve"> C7, C4</t>
-  </si>
-  <si>
-    <t>C11</t>
-  </si>
-  <si>
     <t>Thick Film Resistors - SMD 0402 1%270ohm</t>
   </si>
   <si>
@@ -296,9 +269,6 @@
     <t>C0402C105K8PAC7411</t>
   </si>
   <si>
-    <t>C0402C475M9PACTU</t>
-  </si>
-  <si>
     <t>MURATA</t>
   </si>
   <si>
@@ -353,9 +323,6 @@
     <t>Multilayer Ceramic Capacitor, 10 uF, 10 V, ± 20%, X5R, 0402 [1005 Metric]</t>
   </si>
   <si>
-    <t>https://octopart.com/c0402c475m9pactu-kemet-65485666?r=sp</t>
-  </si>
-  <si>
     <t>https://octopart.com/c0402c105k8pac7411-kemet-75146233?r=sp</t>
   </si>
   <si>
@@ -371,9 +338,6 @@
     <t>https://octopart.com/ac0402fr-7w47kl-yageo-96301082?r=sp</t>
   </si>
   <si>
-    <t>Multilayer Ceramic Capacitor, 4.7 uF, 6.3 V, ± 20%, X5R, 0402</t>
-  </si>
-  <si>
     <t>Power Distribution Load Switch IC</t>
   </si>
   <si>
@@ -390,6 +354,30 @@
   </si>
   <si>
     <t xml:space="preserve">VL53L8 IR ToF LiDar Sensor (H08R6) </t>
+  </si>
+  <si>
+    <t>Multilayer Ceramic Capacitors MLCC - SMD/SMT 0603 25V 4.7uF X5R 10% T: 0.8mm</t>
+  </si>
+  <si>
+    <t>C1608X5R1E475K080AC</t>
+  </si>
+  <si>
+    <t>https://octopart.com/c1608x5r1e475k080ac-tdk-26013502?r=sp</t>
+  </si>
+  <si>
+    <t>C11, C7, C4</t>
+  </si>
+  <si>
+    <t>Ind chip Bead Multi-Layer 30 ohms 25% 100MHZ Ferrite 1,5A 0603Punched paper T/R</t>
+  </si>
+  <si>
+    <t>MMZ1608Y300BTA00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TDK </t>
+  </si>
+  <si>
+    <t>https://octopart.com/mmz1608y300bta00-tdk-7906990?r=sp</t>
   </si>
 </sst>
 </file>
@@ -703,9 +691,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2277741</xdr:colOff>
+      <xdr:colOff>2275836</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>20002</xdr:rowOff>
+      <xdr:rowOff>16192</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1043,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1135,7 +1123,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
@@ -1170,16 +1158,16 @@
         <v>18</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>47</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>50</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F9" s="19">
         <v>1</v>
@@ -1190,7 +1178,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>21</v>
@@ -1207,19 +1195,19 @@
     </row>
     <row r="11" spans="1:9" s="16" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F11" s="19">
         <v>11</v>
@@ -1227,19 +1215,19 @@
     </row>
     <row r="12" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="F12" s="19">
         <v>1</v>
@@ -1250,76 +1238,76 @@
         <v>40</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F13" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
-        <v>70</v>
+      <c r="A14" s="17" t="s">
+        <v>109</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>86</v>
+        <v>107</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="F14" s="19">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="F15" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>104</v>
+        <v>49</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>88</v>
+        <v>50</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>103</v>
+        <v>51</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="F16" s="19">
         <v>1</v>
@@ -1327,19 +1315,19 @@
     </row>
     <row r="17" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F17" s="19">
         <v>1</v>
@@ -1347,99 +1335,99 @@
     </row>
     <row r="18" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="F18" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="F19" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="16" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="F20" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="16" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="F21" s="19">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="18" t="s">
         <v>113</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>116</v>
       </c>
       <c r="F22" s="19">
         <v>1</v>
@@ -1447,19 +1435,19 @@
     </row>
     <row r="23" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D23" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="18" t="s">
         <v>43</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>46</v>
       </c>
       <c r="F23" s="19">
         <v>1</v>
@@ -1467,39 +1455,39 @@
     </row>
     <row r="24" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="F24" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
-        <v>26</v>
+      <c r="A25" s="21" t="s">
+        <v>41</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>28</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>29</v>
+        <v>86</v>
       </c>
       <c r="F25" s="19">
         <v>1</v>
@@ -1507,19 +1495,19 @@
     </row>
     <row r="26" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>28</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F26" s="19">
         <v>1</v>
@@ -1527,19 +1515,19 @@
     </row>
     <row r="27" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>28</v>
+        <v>89</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F27" s="19">
         <v>1</v>
@@ -1547,61 +1535,41 @@
     </row>
     <row r="28" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="F28" s="19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
-        <v>84</v>
+      <c r="A29" s="17" t="s">
+        <v>32</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>101</v>
+        <v>35</v>
       </c>
       <c r="F29" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="F30" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1612,21 +1580,21 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E25" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E30" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D24" r:id="rId3" display="https://octopart.com/manufacturers/wolfspeed" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E24" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E29" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D23" r:id="rId3" display="https://octopart.com/manufacturers/wolfspeed" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="E10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E23" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E24" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E17" r:id="rId7" display="https://octopart.com/rc0603jr-070rl-yageo-1241539?r=sp" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E11" r:id="rId8" display="https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp&amp;s=9bS9ASSwSEqMCE9KBEQZ0g" xr:uid="{663B604C-0778-4D31-8D01-1E3B83AE8D9B}"/>
-    <hyperlink ref="E13" r:id="rId9" display="https://octopart.com/cc0805kkx7r7bb105-yageo-8376555?r=sp" xr:uid="{636BB640-56DA-4B3A-8EBB-00A74F7EF75D}"/>
-    <hyperlink ref="E15" r:id="rId10" display="https://octopart.com/10tpu4r7msi-panasonic-29487748?r=sp" xr:uid="{23CC8D52-00B7-424D-AE6F-D90CF0F8A6D7}"/>
-    <hyperlink ref="E18" r:id="rId11" display="https://octopart.com/erj-3geyj271v-panasonic-55560546" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E19" r:id="rId12" display="https://octopart.com/search?q=060300F2201T5E&amp;currency=USD&amp;specs=0" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E20" r:id="rId13" display="https://octopart.com/search?q=RC0603FR-0710KL&amp;currency=USD&amp;specs=0" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E9" r:id="rId14" display="https://octopart.com/87227-1-te+connectivity-39512052?r=sp" xr:uid="{97DC24F0-08CA-4316-A0CB-F81F9DEADBAB}"/>
-    <hyperlink ref="E16" r:id="rId15" xr:uid="{1CA08D75-7CE2-4798-BFB4-4DFC1825B006}"/>
+    <hyperlink ref="E23" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E16" r:id="rId6" display="https://octopart.com/rc0603jr-070rl-yageo-1241539?r=sp" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E11" r:id="rId7" display="https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp&amp;s=9bS9ASSwSEqMCE9KBEQZ0g" xr:uid="{663B604C-0778-4D31-8D01-1E3B83AE8D9B}"/>
+    <hyperlink ref="E13" r:id="rId8" display="https://octopart.com/cc0805kkx7r7bb105-yageo-8376555?r=sp" xr:uid="{636BB640-56DA-4B3A-8EBB-00A74F7EF75D}"/>
+    <hyperlink ref="E17" r:id="rId9" display="https://octopart.com/erj-3geyj271v-panasonic-55560546" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E18" r:id="rId10" display="https://octopart.com/search?q=060300F2201T5E&amp;currency=USD&amp;specs=0" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E19" r:id="rId11" display="https://octopart.com/search?q=RC0603FR-0710KL&amp;currency=USD&amp;specs=0" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E9" r:id="rId12" display="https://octopart.com/87227-1-te+connectivity-39512052?r=sp" xr:uid="{97DC24F0-08CA-4316-A0CB-F81F9DEADBAB}"/>
+    <hyperlink ref="E15" r:id="rId13" xr:uid="{1CA08D75-7CE2-4798-BFB4-4DFC1825B006}"/>
+    <hyperlink ref="E14" r:id="rId14" display="https://octopart.com/10tpu4r7msi-panasonic-29487748?r=sp" xr:uid="{23CC8D52-00B7-424D-AE6F-D90CF0F8A6D7}"/>
+    <hyperlink ref="E22" r:id="rId15" display="https://octopart.com/search?q=MPZ1608S601ATD25&amp;currency=USD&amp;specs=0" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId16"/>

</xml_diff>

<commit_message>
-Change the MCU footprint to STM32G0B1CEU6
</commit_message>
<xml_diff>
--- a/Released/BOM/H08R6.xlsx
+++ b/Released/BOM/H08R6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H08R6x-Hardware\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moazzen\Documents\H08R6x-Hardware\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB5EB02-3C36-441B-8120-BB89B7779B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17FA2F8-D683-4A06-922D-62512715E87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H08R6" sheetId="1" r:id="rId1"/>
@@ -215,9 +215,6 @@
     <t>https://octopart.com/grm188r61a105ka61j-murata-9221870?r=sp</t>
   </si>
   <si>
-    <t>C1, C3, C5, C6, C8, C9, C10, C14, C15, C16, C17</t>
-  </si>
-  <si>
     <t>C13</t>
   </si>
   <si>
@@ -365,9 +362,6 @@
     <t>https://octopart.com/c1608x5r1e475k080ac-tdk-26013502?r=sp</t>
   </si>
   <si>
-    <t>C11, C7, C4</t>
-  </si>
-  <si>
     <t>Ind chip Bead Multi-Layer 30 ohms 25% 100MHZ Ferrite 1,5A 0603Punched paper T/R</t>
   </si>
   <si>
@@ -378,6 +372,12 @@
   </si>
   <si>
     <t>https://octopart.com/mmz1608y300bta00-tdk-7906990?r=sp</t>
+  </si>
+  <si>
+    <t>C1, C5, C6, C8, C9, C10, C14, C15, C16, C17</t>
+  </si>
+  <si>
+    <t>C11, C7</t>
   </si>
 </sst>
 </file>
@@ -691,7 +691,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>2275836</xdr:colOff>
+      <xdr:colOff>2270121</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>16192</xdr:rowOff>
     </xdr:to>
@@ -1033,8 +1033,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1112,7 +1112,7 @@
         <v>12</v>
       </c>
       <c r="D5" s="23">
-        <v>45311</v>
+        <v>45637</v>
       </c>
       <c r="E5" s="24"/>
       <c r="F5" s="25"/>
@@ -1123,7 +1123,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
@@ -1193,9 +1193,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="16" customFormat="1" ht="52.8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="16" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>59</v>
+        <v>112</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>53</v>
@@ -1210,24 +1210,24 @@
         <v>55</v>
       </c>
       <c r="F11" s="19">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>61</v>
-      </c>
       <c r="C12" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>46</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F12" s="19">
         <v>1</v>
@@ -1244,7 +1244,7 @@
         <v>57</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E13" s="18" t="s">
         <v>58</v>
@@ -1255,39 +1255,39 @@
     </row>
     <row r="14" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="B14" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="17" t="s">
         <v>106</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>107</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F14" s="19">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F15" s="19">
         <v>1</v>
@@ -1318,16 +1318,16 @@
         <v>36</v>
       </c>
       <c r="B17" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="17" t="s">
         <v>62</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>63</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F17" s="19">
         <v>1</v>
@@ -1338,16 +1338,16 @@
         <v>37</v>
       </c>
       <c r="B18" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>65</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>66</v>
       </c>
       <c r="D18" s="17" t="s">
         <v>51</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F18" s="19">
         <v>2</v>
@@ -1355,19 +1355,19 @@
     </row>
     <row r="19" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="17" t="s">
         <v>68</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>69</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>51</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="19">
         <v>3</v>
@@ -1375,19 +1375,19 @@
     </row>
     <row r="20" spans="1:6" s="16" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>51</v>
       </c>
       <c r="E20" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F20" s="19">
         <v>6</v>
@@ -1395,19 +1395,19 @@
     </row>
     <row r="21" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="17" t="s">
         <v>101</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>102</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>51</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F21" s="19">
         <v>1</v>
@@ -1418,16 +1418,16 @@
         <v>24</v>
       </c>
       <c r="B22" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="E22" s="18" t="s">
         <v>111</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>112</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>113</v>
       </c>
       <c r="F22" s="19">
         <v>1</v>
@@ -1478,16 +1478,16 @@
         <v>41</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>28</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F25" s="19">
         <v>1</v>
@@ -1495,19 +1495,19 @@
     </row>
     <row r="26" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D26" s="17" t="s">
         <v>28</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F26" s="19">
         <v>1</v>
@@ -1515,19 +1515,19 @@
     </row>
     <row r="27" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F27" s="19">
         <v>1</v>
@@ -1535,19 +1535,19 @@
     </row>
     <row r="28" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D28" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E28" s="18" t="s">
         <v>90</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>91</v>
       </c>
       <c r="F28" s="19">
         <v>2</v>

</xml_diff>

<commit_message>
Add the TVS to the BOM
</commit_message>
<xml_diff>
--- a/Released/BOM/H08R6.xlsx
+++ b/Released/BOM/H08R6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moazzen\Documents\H08R6x-Hardware\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B49D552-38C2-440F-B742-6092C88EB6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9B2BE99-A6FF-49D4-AD90-84203D99248E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="119">
   <si>
     <t>Description</t>
   </si>
@@ -113,21 +113,12 @@
     <t>FB1</t>
   </si>
   <si>
-    <t>STM32G0B1CEU6N</t>
-  </si>
-  <si>
     <t>U1</t>
   </si>
   <si>
-    <t>MCU 32-Bit ARM Cortex-M0+ RISC 512kByte Flash 1.7V to 3.6V 48-Pin UFQFPN Tray</t>
-  </si>
-  <si>
     <t>STMicroelectronics</t>
   </si>
   <si>
-    <t>https://octopart.com/stm32g0b1ceu6n-stmicroelectronics-116364672?r=sp</t>
-  </si>
-  <si>
     <t>D1</t>
   </si>
   <si>
@@ -378,6 +369,30 @@
   </si>
   <si>
     <t>C11, C7</t>
+  </si>
+  <si>
+    <t>TVS DIODE 3,3V 10,9V SOD323</t>
+  </si>
+  <si>
+    <t>CDSOD323-T03SC</t>
+  </si>
+  <si>
+    <t>BOURNS INC</t>
+  </si>
+  <si>
+    <t>https://octopart.com/cdsod323-t03sc-bourns-10487153?r=sp</t>
+  </si>
+  <si>
+    <t>MCU 32-bit ARM Cortex M0+ RISC 512KB Flash 1.8V/2.5V/3.3V 48-Pin UFQFPN EP Tray</t>
+  </si>
+  <si>
+    <t>STM32G0B1CEU6</t>
+  </si>
+  <si>
+    <t>https://octopart.com/stm32g0b1ceu6-stmicroelectronics-116363364?r=sp</t>
+  </si>
+  <si>
+    <t>D2</t>
   </si>
 </sst>
 </file>
@@ -576,7 +591,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -655,6 +670,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1031,10 +1049,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1106,7 +1124,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
@@ -1123,7 +1141,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
@@ -1158,16 +1176,16 @@
         <v>18</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>44</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>47</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>19</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F9" s="19">
         <v>1</v>
@@ -1178,7 +1196,7 @@
         <v>20</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>21</v>
@@ -1195,19 +1213,19 @@
     </row>
     <row r="11" spans="1:9" s="16" customFormat="1" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F11" s="19">
         <v>10</v>
@@ -1215,19 +1233,19 @@
     </row>
     <row r="12" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F12" s="19">
         <v>1</v>
@@ -1235,19 +1253,19 @@
     </row>
     <row r="13" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F13" s="19">
         <v>1</v>
@@ -1255,19 +1273,19 @@
     </row>
     <row r="14" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="F14" s="19">
         <v>2</v>
@@ -1275,19 +1293,19 @@
     </row>
     <row r="15" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F15" s="19">
         <v>1</v>
@@ -1298,16 +1316,16 @@
         <v>23</v>
       </c>
       <c r="B16" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>52</v>
       </c>
       <c r="F16" s="19">
         <v>1</v>
@@ -1315,19 +1333,19 @@
     </row>
     <row r="17" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B17" s="17" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>16</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F17" s="19">
         <v>1</v>
@@ -1335,19 +1353,19 @@
     </row>
     <row r="18" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F18" s="19">
         <v>2</v>
@@ -1355,19 +1373,19 @@
     </row>
     <row r="19" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E19" s="18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F19" s="19">
         <v>3</v>
@@ -1375,19 +1393,19 @@
     </row>
     <row r="20" spans="1:6" s="16" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="18" t="s">
         <v>95</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>96</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="F20" s="19">
         <v>6</v>
@@ -1395,19 +1413,19 @@
     </row>
     <row r="21" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="18" t="s">
         <v>100</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>103</v>
       </c>
       <c r="F21" s="19">
         <v>1</v>
@@ -1418,16 +1436,16 @@
         <v>24</v>
       </c>
       <c r="B22" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="18" t="s">
         <v>108</v>
-      </c>
-      <c r="C22" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>111</v>
       </c>
       <c r="F22" s="19">
         <v>1</v>
@@ -1435,19 +1453,19 @@
     </row>
     <row r="23" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>17</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F23" s="19">
         <v>1</v>
@@ -1455,59 +1473,59 @@
     </row>
     <row r="24" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>26</v>
+        <v>118</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>27</v>
+        <v>111</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>25</v>
+        <v>112</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>28</v>
+        <v>113</v>
       </c>
       <c r="E24" s="18" t="s">
-        <v>29</v>
+        <v>114</v>
       </c>
       <c r="F24" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
-        <v>41</v>
+      <c r="A25" s="17" t="s">
+        <v>25</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E25" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="F25" s="19">
+        <v>117</v>
+      </c>
+      <c r="F25" s="29">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>72</v>
+        <v>38</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D26" s="17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E26" s="18" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F26" s="19">
         <v>1</v>
@@ -1515,19 +1533,19 @@
     </row>
     <row r="27" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="E27" s="18" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F27" s="19">
         <v>1</v>
@@ -1535,41 +1553,61 @@
     </row>
     <row r="28" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="21" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B28" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D28" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>90</v>
-      </c>
       <c r="F28" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+    <row r="30" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="F29" s="19">
+      <c r="F30" s="19">
         <v>1</v>
       </c>
     </row>
@@ -1580,21 +1618,21 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E24" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E29" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D23" r:id="rId3" display="https://octopart.com/manufacturers/wolfspeed" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E23" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E16" r:id="rId6" display="https://octopart.com/rc0603jr-070rl-yageo-1241539?r=sp" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E11" r:id="rId7" display="https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp&amp;s=9bS9ASSwSEqMCE9KBEQZ0g" xr:uid="{663B604C-0778-4D31-8D01-1E3B83AE8D9B}"/>
-    <hyperlink ref="E13" r:id="rId8" display="https://octopart.com/cc0805kkx7r7bb105-yageo-8376555?r=sp" xr:uid="{636BB640-56DA-4B3A-8EBB-00A74F7EF75D}"/>
-    <hyperlink ref="E17" r:id="rId9" display="https://octopart.com/erj-3geyj271v-panasonic-55560546" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E18" r:id="rId10" display="https://octopart.com/search?q=060300F2201T5E&amp;currency=USD&amp;specs=0" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E19" r:id="rId11" display="https://octopart.com/search?q=RC0603FR-0710KL&amp;currency=USD&amp;specs=0" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E9" r:id="rId12" display="https://octopart.com/87227-1-te+connectivity-39512052?r=sp" xr:uid="{97DC24F0-08CA-4316-A0CB-F81F9DEADBAB}"/>
-    <hyperlink ref="E15" r:id="rId13" xr:uid="{1CA08D75-7CE2-4798-BFB4-4DFC1825B006}"/>
-    <hyperlink ref="E14" r:id="rId14" display="https://octopart.com/10tpu4r7msi-panasonic-29487748?r=sp" xr:uid="{23CC8D52-00B7-424D-AE6F-D90CF0F8A6D7}"/>
-    <hyperlink ref="E22" r:id="rId15" display="https://octopart.com/search?q=MPZ1608S601ATD25&amp;currency=USD&amp;specs=0" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E30" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D23" r:id="rId2" display="https://octopart.com/manufacturers/wolfspeed" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E10" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E23" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E16" r:id="rId5" display="https://octopart.com/rc0603jr-070rl-yageo-1241539?r=sp" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E11" r:id="rId6" display="https://octopart.com/c0603c104k8ractu-kemet-145075?r=sp&amp;s=9bS9ASSwSEqMCE9KBEQZ0g" xr:uid="{663B604C-0778-4D31-8D01-1E3B83AE8D9B}"/>
+    <hyperlink ref="E13" r:id="rId7" display="https://octopart.com/cc0805kkx7r7bb105-yageo-8376555?r=sp" xr:uid="{636BB640-56DA-4B3A-8EBB-00A74F7EF75D}"/>
+    <hyperlink ref="E17" r:id="rId8" display="https://octopart.com/erj-3geyj271v-panasonic-55560546" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E18" r:id="rId9" display="https://octopart.com/search?q=060300F2201T5E&amp;currency=USD&amp;specs=0" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E19" r:id="rId10" display="https://octopart.com/search?q=RC0603FR-0710KL&amp;currency=USD&amp;specs=0" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E9" r:id="rId11" display="https://octopart.com/87227-1-te+connectivity-39512052?r=sp" xr:uid="{97DC24F0-08CA-4316-A0CB-F81F9DEADBAB}"/>
+    <hyperlink ref="E15" r:id="rId12" xr:uid="{1CA08D75-7CE2-4798-BFB4-4DFC1825B006}"/>
+    <hyperlink ref="E14" r:id="rId13" display="https://octopart.com/10tpu4r7msi-panasonic-29487748?r=sp" xr:uid="{23CC8D52-00B7-424D-AE6F-D90CF0F8A6D7}"/>
+    <hyperlink ref="E22" r:id="rId14" display="https://octopart.com/search?q=MPZ1608S601ATD25&amp;currency=USD&amp;specs=0" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E25" r:id="rId15" xr:uid="{E6D978CB-2525-4C18-9A95-D4D05E7E61DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId16"/>

</xml_diff>